<commit_message>
prepare some basic descriptive plots
</commit_message>
<xml_diff>
--- a/data/raw-data/saa-abstracts-tally.xlsx
+++ b/data/raw-data/saa-abstracts-tally.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Desktop/2020 Spring ARCHY 509/saa-topicmodel/data/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946F9393-9431-A047-9534-41CF89C6DF53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8FA51E-51A4-654F-8D6C-DC04EEF97178}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15100" yWindow="460" windowWidth="13100" windowHeight="17040" xr2:uid="{494A5A0B-14BC-7E4B-868A-FB1F30BF54D3}"/>
+    <workbookView xWindow="2820" yWindow="640" windowWidth="12520" windowHeight="17040" xr2:uid="{494A5A0B-14BC-7E4B-868A-FB1F30BF54D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="14">
   <si>
     <t>year</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>double</t>
+  </si>
+  <si>
+    <t>number_of_abstracts</t>
   </si>
 </sst>
 </file>
@@ -421,21 +424,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888FA89F-180B-E241-91AD-66E159D3673A}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,8 +458,11 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1948</v>
       </c>
@@ -463,37 +470,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1949</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1950</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1951</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1952</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1953</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1954</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1955</v>
       </c>
@@ -501,7 +508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1956</v>
       </c>
@@ -509,7 +516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1957</v>
       </c>
@@ -517,7 +524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1958</v>
       </c>
@@ -525,12 +532,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1959</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1960</v>
       </c>
@@ -538,7 +545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1961</v>
       </c>
@@ -546,7 +553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1962</v>
       </c>
@@ -1092,52 +1099,52 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1995</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1996</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1997</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1998</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1999</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2000</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2001</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2002</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2003</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2004</v>
       </c>
@@ -1147,8 +1154,11 @@
       <c r="C58" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2005</v>
       </c>
@@ -1158,8 +1168,11 @@
       <c r="C59" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2006</v>
       </c>
@@ -1169,8 +1182,11 @@
       <c r="C60" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>2608</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2007</v>
       </c>
@@ -1180,8 +1196,11 @@
       <c r="C61" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>2526</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2008</v>
       </c>
@@ -1191,8 +1210,11 @@
       <c r="C62" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>3441</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2009</v>
       </c>
@@ -1202,8 +1224,11 @@
       <c r="C63" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>2378</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2010</v>
       </c>
@@ -1213,8 +1238,11 @@
       <c r="C64" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G64">
+        <v>3305</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2011</v>
       </c>
@@ -1224,8 +1252,11 @@
       <c r="C65" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2012</v>
       </c>
@@ -1235,8 +1266,11 @@
       <c r="C66" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G66">
+        <v>3440</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2013</v>
       </c>
@@ -1246,8 +1280,11 @@
       <c r="C67" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G67">
+        <v>3255</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2014</v>
       </c>
@@ -1257,8 +1294,11 @@
       <c r="C68" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G68">
+        <v>4047</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2015</v>
       </c>
@@ -1268,8 +1308,11 @@
       <c r="C69" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G69">
+        <v>4797</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2016</v>
       </c>
@@ -1279,8 +1322,11 @@
       <c r="C70" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G70">
+        <v>3426</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2017</v>
       </c>
@@ -1290,8 +1336,11 @@
       <c r="C71" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G71">
+        <v>4722</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2018</v>
       </c>
@@ -1301,8 +1350,11 @@
       <c r="C72" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G72">
+        <v>4173</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2019</v>
       </c>
@@ -1312,8 +1364,11 @@
       <c r="C73" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G73">
+        <v>4464</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2020</v>
       </c>
@@ -1322,6 +1377,9 @@
       </c>
       <c r="C74" t="s">
         <v>9</v>
+      </c>
+      <c r="G74">
+        <v>3150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update abstract number for early years
</commit_message>
<xml_diff>
--- a/data/raw-data/saa-abstracts-tally.xlsx
+++ b/data/raw-data/saa-abstracts-tally.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Desktop/2020 Spring ARCHY 509/saa-topicmodel/data/raw-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/Archy509_2020/saa-topicmodel/data/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8FA51E-51A4-654F-8D6C-DC04EEF97178}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88399E39-1F13-6440-9554-0FCF64FEA46C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="640" windowWidth="12520" windowHeight="17040" xr2:uid="{494A5A0B-14BC-7E4B-868A-FB1F30BF54D3}"/>
+    <workbookView xWindow="2820" yWindow="460" windowWidth="19320" windowHeight="16260" xr2:uid="{494A5A0B-14BC-7E4B-868A-FB1F30BF54D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888FA89F-180B-E241-91AD-66E159D3673A}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="93" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,8 +572,11 @@
       <c r="F16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1963</v>
       </c>
@@ -581,7 +584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1964</v>
       </c>
@@ -600,8 +603,11 @@
       <c r="F18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1965</v>
       </c>
@@ -609,7 +615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1966</v>
       </c>
@@ -617,12 +623,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1967</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1968</v>
       </c>
@@ -630,7 +636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1969</v>
       </c>
@@ -649,8 +655,11 @@
       <c r="F23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1970</v>
       </c>
@@ -658,7 +667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1971</v>
       </c>
@@ -666,7 +675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1972</v>
       </c>
@@ -685,8 +694,11 @@
       <c r="F26" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1973</v>
       </c>
@@ -705,8 +717,11 @@
       <c r="F27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1974</v>
       </c>
@@ -725,8 +740,11 @@
       <c r="F28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1975</v>
       </c>
@@ -745,8 +763,11 @@
       <c r="F29" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1976</v>
       </c>
@@ -765,8 +786,11 @@
       <c r="F30" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1977</v>
       </c>
@@ -785,8 +809,11 @@
       <c r="F31" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1978</v>
       </c>
@@ -805,8 +832,11 @@
       <c r="F32" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1979</v>
       </c>
@@ -825,8 +855,11 @@
       <c r="F33" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1980</v>
       </c>
@@ -845,8 +878,11 @@
       <c r="F34" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1981</v>
       </c>
@@ -854,7 +890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1982</v>
       </c>
@@ -873,8 +909,11 @@
       <c r="F36" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1983</v>
       </c>
@@ -893,8 +932,11 @@
       <c r="F37" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1984</v>
       </c>
@@ -913,8 +955,11 @@
       <c r="F38" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1985</v>
       </c>
@@ -933,8 +978,11 @@
       <c r="F39" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1986</v>
       </c>
@@ -953,8 +1001,11 @@
       <c r="F40" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1987</v>
       </c>
@@ -973,8 +1024,11 @@
       <c r="F41" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1988</v>
       </c>
@@ -993,8 +1047,11 @@
       <c r="F42" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1989</v>
       </c>
@@ -1013,8 +1070,11 @@
       <c r="F43" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1990</v>
       </c>
@@ -1033,13 +1093,16 @@
       <c r="F44" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1991</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1992</v>
       </c>
@@ -1058,8 +1121,11 @@
       <c r="F46" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1993</v>
       </c>
@@ -1078,8 +1144,11 @@
       <c r="F47" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1994</v>
       </c>
@@ -1097,6 +1166,9 @@
       </c>
       <c r="F48" t="s">
         <v>12</v>
+      </c>
+      <c r="G48">
+        <v>801</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix 1985 text, which had a problem with PDF -> PNG conversion
</commit_message>
<xml_diff>
--- a/data/raw-data/saa-abstracts-tally.xlsx
+++ b/data/raw-data/saa-abstracts-tally.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/Archy509_2020/saa-topicmodel/data/raw-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Desktop/2020 Spring ARCHY 509/saa-topicmodel/data/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88399E39-1F13-6440-9554-0FCF64FEA46C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E3AC31-B9FF-9048-BF83-915492FB32D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2820" yWindow="460" windowWidth="19320" windowHeight="16260" xr2:uid="{494A5A0B-14BC-7E4B-868A-FB1F30BF54D3}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="93" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -970,7 +970,7 @@
         <v>5</v>
       </c>
       <c r="D39">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E39">
         <v>79</v>

</xml_diff>